<commit_message>
Fixed error to KargvaDatabase.h
</commit_message>
<xml_diff>
--- a/extracted_SNP_files/metamarcSNPinfo_final.xlsx
+++ b/extracted_SNP_files/metamarcSNPinfo_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AmrPlusPlus_SNP\extracted_SNP_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC65A730-CA21-4C93-AD86-3B7A2F453F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BB37B5-7DC0-4D0B-B2F6-83307ED45A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3820,15 +3820,6 @@
     <t>Mult:Reg:L430R_FGTSQ_SQFMD;Reg:D435V_LSQFM_QNNPL</t>
   </si>
   <si>
-    <t>Del:S431-_GTSQL_QFMDQ</t>
-  </si>
-  <si>
-    <t>Del:Q432-_TSQLS_FMDQN</t>
-  </si>
-  <si>
-    <t>Del:M434-_QLSQF_DQNNP</t>
-  </si>
-  <si>
     <t>Mult:Reg:D435Y_LSQFM_QNNPL;Reg:L430R_FGTSQ_SQFMD</t>
   </si>
   <si>
@@ -3844,12 +3835,6 @@
     <t>Mult:Reg:D435Y_LSQFM_QNNPL;Reg:L490V_GPNIG_IGSLS</t>
   </si>
   <si>
-    <t>Del:N438-_FMDQN_PLSGL</t>
-  </si>
-  <si>
-    <t>Del:L443-_NPLSG_THKRR</t>
-  </si>
-  <si>
     <t>Mult:Reg:H445P_LSGLT_KRRLS;Reg:K446Q_SGLTH_RRLSA</t>
   </si>
   <si>
@@ -4298,6 +4283,21 @@
   </si>
   <si>
     <t>Reg:T451A_EYSSN_YMVQT</t>
+  </si>
+  <si>
+    <t>Mult:Del:S431-_GTSQL_QFMDQ;Del:Q432-_TSQLS_FMDQN;Del:F433-_SQLSQ_MDQNN;Reg:H445Q_LSGLT_KRRLS</t>
+  </si>
+  <si>
+    <t>Mult:Reg:Q432H_TSQLS_FMDQN;Del:F433-_SQLSQ_MDQNN;Del:M434-_QLSQF_DQNNP;Del:D435-_LSQFM_QNNPL</t>
+  </si>
+  <si>
+    <t>Mult:Del:M434-_QLSQF_DQNNP;Del:D435-_LSQFM_QNNPL;Del:Q436-_SQFMD_NNPLS;Del:N437-_QFMDQ_NPLSG</t>
+  </si>
+  <si>
+    <t>Mult:Del:N438-_FMDQN_PLSGL;Reg:S441L_QNNPL_GLTHK;Reg:S450L_HKRRL_ALGPG</t>
+  </si>
+  <si>
+    <t>Mult:Reg:L443W_NPLSG_THKRR;Reg:T444P_PLSGL_HKRRL;Reg:H445Q_LSGLT_KRRLS;Del:K446-_SGLTH_RRLSA</t>
   </si>
 </sst>
 </file>
@@ -5140,8 +5140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A169" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:XFD130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10764,7 +10764,7 @@
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>1421</v>
+        <v>1416</v>
       </c>
       <c r="B185" t="s">
         <v>1</v>
@@ -10776,16 +10776,16 @@
         <v>256</v>
       </c>
       <c r="E185" t="s">
-        <v>1422</v>
+        <v>1417</v>
       </c>
       <c r="F185" t="s">
-        <v>1423</v>
+        <v>1418</v>
       </c>
       <c r="G185" t="s">
-        <v>1424</v>
+        <v>1419</v>
       </c>
       <c r="H185" t="s">
-        <v>1425</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.3">
@@ -11494,156 +11494,156 @@
         <v>1265</v>
       </c>
       <c r="Z199" t="s">
+        <v>1421</v>
+      </c>
+      <c r="AA199" t="s">
+        <v>1422</v>
+      </c>
+      <c r="AB199" t="s">
+        <v>1423</v>
+      </c>
+      <c r="AC199" t="s">
         <v>1266</v>
       </c>
-      <c r="AA199" t="s">
+      <c r="AD199" t="s">
         <v>1267</v>
       </c>
-      <c r="AB199" t="s">
+      <c r="AE199" t="s">
         <v>1268</v>
       </c>
-      <c r="AC199" t="s">
+      <c r="AF199" t="s">
         <v>1269</v>
       </c>
-      <c r="AD199" t="s">
+      <c r="AG199" t="s">
         <v>1270</v>
       </c>
-      <c r="AE199" t="s">
+      <c r="AH199" t="s">
+        <v>1424</v>
+      </c>
+      <c r="AI199" t="s">
+        <v>1425</v>
+      </c>
+      <c r="AJ199" t="s">
         <v>1271</v>
       </c>
-      <c r="AF199" t="s">
+      <c r="AK199" t="s">
         <v>1272</v>
       </c>
-      <c r="AG199" t="s">
+      <c r="AL199" t="s">
         <v>1273</v>
       </c>
-      <c r="AH199" t="s">
+      <c r="AM199" t="s">
         <v>1274</v>
       </c>
-      <c r="AI199" t="s">
+      <c r="AN199" t="s">
         <v>1275</v>
       </c>
-      <c r="AJ199" t="s">
+      <c r="AO199" t="s">
         <v>1276</v>
       </c>
-      <c r="AK199" t="s">
+      <c r="AP199" t="s">
         <v>1277</v>
       </c>
-      <c r="AL199" t="s">
+      <c r="AQ199" t="s">
         <v>1278</v>
       </c>
-      <c r="AM199" t="s">
+      <c r="AR199" t="s">
         <v>1279</v>
       </c>
-      <c r="AN199" t="s">
+      <c r="AS199" t="s">
         <v>1280</v>
       </c>
-      <c r="AO199" t="s">
+      <c r="AT199" t="s">
         <v>1281</v>
       </c>
-      <c r="AP199" t="s">
+      <c r="AU199" t="s">
         <v>1282</v>
       </c>
-      <c r="AQ199" t="s">
+      <c r="AV199" t="s">
         <v>1283</v>
       </c>
-      <c r="AR199" t="s">
+      <c r="AW199" t="s">
         <v>1284</v>
       </c>
-      <c r="AS199" t="s">
+      <c r="AX199" t="s">
         <v>1285</v>
       </c>
-      <c r="AT199" t="s">
+      <c r="AY199" t="s">
         <v>1286</v>
       </c>
-      <c r="AU199" t="s">
+      <c r="AZ199" t="s">
         <v>1287</v>
       </c>
-      <c r="AV199" t="s">
+      <c r="BA199" t="s">
         <v>1288</v>
       </c>
-      <c r="AW199" t="s">
+      <c r="BB199" t="s">
         <v>1289</v>
       </c>
-      <c r="AX199" t="s">
+      <c r="BC199" t="s">
         <v>1290</v>
       </c>
-      <c r="AY199" t="s">
+      <c r="BD199" t="s">
         <v>1291</v>
       </c>
-      <c r="AZ199" t="s">
+      <c r="BE199" t="s">
         <v>1292</v>
       </c>
-      <c r="BA199" t="s">
+      <c r="BF199" t="s">
         <v>1293</v>
       </c>
-      <c r="BB199" t="s">
+      <c r="BG199" t="s">
         <v>1294</v>
       </c>
-      <c r="BC199" t="s">
+      <c r="BH199" t="s">
         <v>1295</v>
       </c>
-      <c r="BD199" t="s">
+      <c r="BI199" t="s">
         <v>1296</v>
       </c>
-      <c r="BE199" t="s">
+      <c r="BJ199" t="s">
         <v>1297</v>
       </c>
-      <c r="BF199" t="s">
+      <c r="BK199" t="s">
         <v>1298</v>
       </c>
-      <c r="BG199" t="s">
+      <c r="BL199" t="s">
         <v>1299</v>
       </c>
-      <c r="BH199" t="s">
+      <c r="BM199" t="s">
         <v>1300</v>
       </c>
-      <c r="BI199" t="s">
+      <c r="BN199" t="s">
         <v>1301</v>
       </c>
-      <c r="BJ199" t="s">
+      <c r="BO199" t="s">
         <v>1302</v>
       </c>
-      <c r="BK199" t="s">
+      <c r="BP199" t="s">
         <v>1303</v>
       </c>
-      <c r="BL199" t="s">
+      <c r="BQ199" t="s">
         <v>1304</v>
       </c>
-      <c r="BM199" t="s">
+      <c r="BR199" t="s">
         <v>1305</v>
       </c>
-      <c r="BN199" t="s">
+      <c r="BS199" t="s">
         <v>1306</v>
       </c>
-      <c r="BO199" t="s">
+      <c r="BT199" t="s">
         <v>1307</v>
       </c>
-      <c r="BP199" t="s">
+      <c r="BU199" t="s">
         <v>1308</v>
       </c>
-      <c r="BQ199" t="s">
+      <c r="BV199" t="s">
         <v>1309</v>
-      </c>
-      <c r="BR199" t="s">
-        <v>1310</v>
-      </c>
-      <c r="BS199" t="s">
-        <v>1311</v>
-      </c>
-      <c r="BT199" t="s">
-        <v>1312</v>
-      </c>
-      <c r="BU199" t="s">
-        <v>1313</v>
-      </c>
-      <c r="BV199" t="s">
-        <v>1314</v>
       </c>
     </row>
     <row r="200" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>1315</v>
+        <v>1310</v>
       </c>
       <c r="B200" t="s">
         <v>1</v>
@@ -11658,15 +11658,15 @@
         <v>148</v>
       </c>
       <c r="F200" t="s">
-        <v>1316</v>
+        <v>1311</v>
       </c>
       <c r="G200" t="s">
-        <v>1317</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="201" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>1318</v>
+        <v>1313</v>
       </c>
       <c r="B201" t="s">
         <v>1</v>
@@ -11705,12 +11705,12 @@
         <v>465</v>
       </c>
       <c r="N201" t="s">
-        <v>1319</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="202" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
       <c r="B202" t="s">
         <v>1</v>
@@ -11725,39 +11725,39 @@
         <v>148</v>
       </c>
       <c r="F202" t="s">
+        <v>1316</v>
+      </c>
+      <c r="G202" t="s">
+        <v>1317</v>
+      </c>
+      <c r="H202" t="s">
+        <v>1318</v>
+      </c>
+      <c r="I202" t="s">
+        <v>1319</v>
+      </c>
+      <c r="J202" t="s">
+        <v>1320</v>
+      </c>
+      <c r="K202" t="s">
         <v>1321</v>
       </c>
-      <c r="G202" t="s">
+      <c r="L202" t="s">
         <v>1322</v>
       </c>
-      <c r="H202" t="s">
+      <c r="M202" t="s">
         <v>1323</v>
       </c>
-      <c r="I202" t="s">
+      <c r="N202" t="s">
         <v>1324</v>
       </c>
-      <c r="J202" t="s">
+      <c r="O202" t="s">
         <v>1325</v>
-      </c>
-      <c r="K202" t="s">
-        <v>1326</v>
-      </c>
-      <c r="L202" t="s">
-        <v>1327</v>
-      </c>
-      <c r="M202" t="s">
-        <v>1328</v>
-      </c>
-      <c r="N202" t="s">
-        <v>1329</v>
-      </c>
-      <c r="O202" t="s">
-        <v>1330</v>
       </c>
     </row>
     <row r="203" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>1331</v>
+        <v>1326</v>
       </c>
       <c r="B203" t="s">
         <v>1</v>
@@ -11783,7 +11783,7 @@
     </row>
     <row r="204" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>1332</v>
+        <v>1327</v>
       </c>
       <c r="B204" t="s">
         <v>1</v>
@@ -11827,7 +11827,7 @@
     </row>
     <row r="205" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>1333</v>
+        <v>1328</v>
       </c>
       <c r="B205" t="s">
         <v>1</v>
@@ -11871,7 +11871,7 @@
     </row>
     <row r="206" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>1334</v>
+        <v>1329</v>
       </c>
       <c r="B206" t="s">
         <v>1</v>
@@ -11897,7 +11897,7 @@
     </row>
     <row r="207" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>1335</v>
+        <v>1330</v>
       </c>
       <c r="B207" t="s">
         <v>1</v>
@@ -11929,7 +11929,7 @@
     </row>
     <row r="208" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>1336</v>
+        <v>1331</v>
       </c>
       <c r="B208" t="s">
         <v>1</v>
@@ -11958,7 +11958,7 @@
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>1337</v>
+        <v>1332</v>
       </c>
       <c r="B209" t="s">
         <v>1</v>
@@ -12002,7 +12002,7 @@
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>1338</v>
+        <v>1333</v>
       </c>
       <c r="B210" t="s">
         <v>1</v>
@@ -12046,7 +12046,7 @@
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>1339</v>
+        <v>1334</v>
       </c>
       <c r="B211" t="s">
         <v>1</v>
@@ -12090,7 +12090,7 @@
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>1340</v>
+        <v>1335</v>
       </c>
       <c r="B212" t="s">
         <v>1</v>
@@ -12119,7 +12119,7 @@
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>1341</v>
+        <v>1336</v>
       </c>
       <c r="B213" t="s">
         <v>1</v>
@@ -12163,7 +12163,7 @@
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>1342</v>
+        <v>1337</v>
       </c>
       <c r="B214" t="s">
         <v>1</v>
@@ -12309,7 +12309,7 @@
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>1343</v>
+        <v>1338</v>
       </c>
       <c r="B218" t="s">
         <v>1</v>
@@ -12397,7 +12397,7 @@
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>1344</v>
+        <v>1339</v>
       </c>
       <c r="B220" t="s">
         <v>1</v>
@@ -12467,7 +12467,7 @@
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>1345</v>
+        <v>1340</v>
       </c>
       <c r="B222" t="s">
         <v>1</v>
@@ -13119,7 +13119,7 @@
     </row>
     <row r="239" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>1346</v>
+        <v>1341</v>
       </c>
       <c r="B239" t="s">
         <v>1</v>
@@ -13128,24 +13128,24 @@
         <v>577</v>
       </c>
       <c r="D239" t="s">
-        <v>1347</v>
+        <v>1342</v>
       </c>
       <c r="E239" t="s">
-        <v>1348</v>
+        <v>1343</v>
       </c>
       <c r="F239" t="s">
-        <v>1349</v>
+        <v>1344</v>
       </c>
       <c r="G239" t="s">
-        <v>1350</v>
+        <v>1345</v>
       </c>
       <c r="H239" t="s">
-        <v>1351</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="240" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>1352</v>
+        <v>1347</v>
       </c>
       <c r="B240" t="s">
         <v>122</v>
@@ -13157,38 +13157,38 @@
         <v>939</v>
       </c>
       <c r="E240" t="s">
-        <v>1353</v>
+        <v>1348</v>
       </c>
       <c r="F240" t="s">
-        <v>1354</v>
+        <v>1349</v>
       </c>
       <c r="G240" t="s">
-        <v>1355</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="241" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>1356</v>
+        <v>1351</v>
       </c>
       <c r="B241" t="s">
         <v>122</v>
       </c>
       <c r="C241" t="s">
-        <v>1357</v>
+        <v>1352</v>
       </c>
       <c r="D241" t="s">
-        <v>1358</v>
+        <v>1353</v>
       </c>
       <c r="E241" t="s">
-        <v>1359</v>
+        <v>1354</v>
       </c>
       <c r="F241" t="s">
-        <v>1360</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="242" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>1361</v>
+        <v>1356</v>
       </c>
       <c r="B242" t="s">
         <v>1</v>
@@ -13200,61 +13200,61 @@
         <v>394</v>
       </c>
       <c r="E242" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F242" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G242" t="s">
+        <v>1359</v>
+      </c>
+      <c r="H242" t="s">
+        <v>1360</v>
+      </c>
+      <c r="I242" t="s">
+        <v>1361</v>
+      </c>
+      <c r="J242" t="s">
         <v>1362</v>
       </c>
-      <c r="F242" t="s">
+      <c r="K242" t="s">
         <v>1363</v>
       </c>
-      <c r="G242" t="s">
+      <c r="L242" t="s">
         <v>1364</v>
       </c>
-      <c r="H242" t="s">
+      <c r="M242" t="s">
         <v>1365</v>
       </c>
-      <c r="I242" t="s">
+      <c r="N242" t="s">
         <v>1366</v>
       </c>
-      <c r="J242" t="s">
+      <c r="O242" t="s">
         <v>1367</v>
       </c>
-      <c r="K242" t="s">
+      <c r="P242" t="s">
         <v>1368</v>
       </c>
-      <c r="L242" t="s">
+      <c r="Q242" t="s">
         <v>1369</v>
       </c>
-      <c r="M242" t="s">
+      <c r="R242" t="s">
         <v>1370</v>
       </c>
-      <c r="N242" t="s">
+      <c r="S242" t="s">
         <v>1371</v>
       </c>
-      <c r="O242" t="s">
+      <c r="T242" t="s">
         <v>1372</v>
       </c>
-      <c r="P242" t="s">
+      <c r="U242" t="s">
         <v>1373</v>
       </c>
-      <c r="Q242" t="s">
+      <c r="V242" t="s">
         <v>1374</v>
       </c>
-      <c r="R242" t="s">
+      <c r="W242" t="s">
         <v>1375</v>
-      </c>
-      <c r="S242" t="s">
-        <v>1376</v>
-      </c>
-      <c r="T242" t="s">
-        <v>1377</v>
-      </c>
-      <c r="U242" t="s">
-        <v>1378</v>
-      </c>
-      <c r="V242" t="s">
-        <v>1379</v>
-      </c>
-      <c r="W242" t="s">
-        <v>1380</v>
       </c>
     </row>
     <row r="243" spans="1:23" x14ac:dyDescent="0.3">
@@ -13373,7 +13373,7 @@
     </row>
     <row r="246" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>1381</v>
+        <v>1376</v>
       </c>
       <c r="B246" t="s">
         <v>1</v>
@@ -13388,30 +13388,30 @@
         <v>683</v>
       </c>
       <c r="F246" t="s">
+        <v>1377</v>
+      </c>
+      <c r="G246" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H246" t="s">
+        <v>1379</v>
+      </c>
+      <c r="I246" t="s">
+        <v>1380</v>
+      </c>
+      <c r="J246" t="s">
+        <v>1381</v>
+      </c>
+      <c r="K246" t="s">
         <v>1382</v>
       </c>
-      <c r="G246" t="s">
+      <c r="L246" t="s">
         <v>1383</v>
-      </c>
-      <c r="H246" t="s">
-        <v>1384</v>
-      </c>
-      <c r="I246" t="s">
-        <v>1385</v>
-      </c>
-      <c r="J246" t="s">
-        <v>1386</v>
-      </c>
-      <c r="K246" t="s">
-        <v>1387</v>
-      </c>
-      <c r="L246" t="s">
-        <v>1388</v>
       </c>
     </row>
     <row r="247" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>1389</v>
+        <v>1384</v>
       </c>
       <c r="B247" t="s">
         <v>1</v>
@@ -13426,10 +13426,10 @@
         <v>683</v>
       </c>
       <c r="F247" t="s">
-        <v>1390</v>
+        <v>1385</v>
       </c>
       <c r="G247" t="s">
-        <v>1391</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="248" spans="1:23" x14ac:dyDescent="0.3">
@@ -13483,7 +13483,7 @@
     </row>
     <row r="250" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>1392</v>
+        <v>1387</v>
       </c>
       <c r="B250" t="s">
         <v>1</v>
@@ -13498,7 +13498,7 @@
         <v>683</v>
       </c>
       <c r="F250" t="s">
-        <v>1393</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="251" spans="1:23" x14ac:dyDescent="0.3">
@@ -13615,7 +13615,7 @@
     </row>
     <row r="253" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>1394</v>
+        <v>1389</v>
       </c>
       <c r="B253" t="s">
         <v>1</v>
@@ -13783,7 +13783,7 @@
     </row>
     <row r="256" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>1395</v>
+        <v>1390</v>
       </c>
       <c r="B256" t="s">
         <v>1</v>
@@ -13836,7 +13836,7 @@
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>1396</v>
+        <v>1391</v>
       </c>
       <c r="B257" t="s">
         <v>1</v>
@@ -14113,7 +14113,7 @@
     </row>
     <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>1397</v>
+        <v>1392</v>
       </c>
       <c r="B262" t="s">
         <v>1</v>
@@ -14166,7 +14166,7 @@
     </row>
     <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>1398</v>
+        <v>1393</v>
       </c>
       <c r="B263" t="s">
         <v>1</v>
@@ -14222,7 +14222,7 @@
     </row>
     <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="B264" t="s">
         <v>1</v>
@@ -14234,27 +14234,27 @@
         <v>88</v>
       </c>
       <c r="E264" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F264" t="s">
+        <v>1396</v>
+      </c>
+      <c r="G264" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H264" t="s">
+        <v>1398</v>
+      </c>
+      <c r="I264" t="s">
+        <v>1399</v>
+      </c>
+      <c r="J264" t="s">
         <v>1400</v>
-      </c>
-      <c r="F264" t="s">
-        <v>1401</v>
-      </c>
-      <c r="G264" t="s">
-        <v>1402</v>
-      </c>
-      <c r="H264" t="s">
-        <v>1403</v>
-      </c>
-      <c r="I264" t="s">
-        <v>1404</v>
-      </c>
-      <c r="J264" t="s">
-        <v>1405</v>
       </c>
     </row>
     <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
       <c r="B265" t="s">
         <v>1</v>
@@ -14266,15 +14266,15 @@
         <v>88</v>
       </c>
       <c r="E265" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="F265" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
       <c r="B266" t="s">
         <v>1</v>
@@ -14283,30 +14283,30 @@
         <v>75</v>
       </c>
       <c r="D266" t="s">
+        <v>1404</v>
+      </c>
+      <c r="E266" t="s">
+        <v>1405</v>
+      </c>
+      <c r="F266" t="s">
+        <v>1406</v>
+      </c>
+      <c r="G266" t="s">
+        <v>1407</v>
+      </c>
+      <c r="H266" t="s">
+        <v>1408</v>
+      </c>
+      <c r="I266" t="s">
         <v>1409</v>
       </c>
-      <c r="E266" t="s">
+      <c r="J266" t="s">
         <v>1410</v>
-      </c>
-      <c r="F266" t="s">
-        <v>1411</v>
-      </c>
-      <c r="G266" t="s">
-        <v>1412</v>
-      </c>
-      <c r="H266" t="s">
-        <v>1413</v>
-      </c>
-      <c r="I266" t="s">
-        <v>1414</v>
-      </c>
-      <c r="J266" t="s">
-        <v>1415</v>
       </c>
     </row>
     <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>1416</v>
+        <v>1411</v>
       </c>
       <c r="B267" t="s">
         <v>1</v>
@@ -14318,16 +14318,16 @@
         <v>3</v>
       </c>
       <c r="E267" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="F267" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="G267" t="s">
-        <v>1419</v>
+        <v>1414</v>
       </c>
       <c r="H267" t="s">
-        <v>1420</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="268" spans="1:18" x14ac:dyDescent="0.3">
@@ -14351,8 +14351,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DO269">
-    <sortCondition ref="A2:A269"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DO267">
+    <sortCondition ref="A2:A267"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed second error in KargvaDatabase
</commit_message>
<xml_diff>
--- a/extracted_SNP_files/metamarcSNPinfo_final.xlsx
+++ b/extracted_SNP_files/metamarcSNPinfo_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AmrPlusPlus_SNP\extracted_SNP_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BB37B5-7DC0-4D0B-B2F6-83307ED45A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA9ED71-D673-48C3-B6AF-0D7187A8DFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2200,9 +2200,6 @@
     <t>OPRD</t>
   </si>
   <si>
-    <t>Reg:Q142X_KWGEM_PTAPV</t>
-  </si>
-  <si>
     <t>MEG_7304</t>
   </si>
   <si>
@@ -4298,6 +4295,9 @@
   </si>
   <si>
     <t>Mult:Reg:L443W_NPLSG_THKRR;Reg:T444P_PLSGL_HKRRL;Reg:H445Q_LSGLT_KRRLS;Del:K446-_SGLTH_RRLSA</t>
+  </si>
+  <si>
+    <t>Non:Q142*_KWGEM_PTAPV</t>
   </si>
 </sst>
 </file>
@@ -5140,8 +5140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:XFD130"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7571,7 +7571,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
@@ -7591,7 +7591,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
@@ -7606,18 +7606,18 @@
         <v>195</v>
       </c>
       <c r="F73" t="s">
+        <v>732</v>
+      </c>
+      <c r="G73" t="s">
         <v>733</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>734</v>
-      </c>
-      <c r="H73" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -7640,7 +7640,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
@@ -7666,7 +7666,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B76" t="s">
         <v>1</v>
@@ -7692,7 +7692,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
@@ -7715,7 +7715,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B78" t="s">
         <v>1</v>
@@ -7738,7 +7738,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
@@ -7764,7 +7764,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
@@ -7790,7 +7790,7 @@
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
@@ -7839,7 +7839,7 @@
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
@@ -7862,7 +7862,7 @@
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
@@ -7914,7 +7914,7 @@
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
@@ -7940,7 +7940,7 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
@@ -7966,7 +7966,7 @@
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
@@ -8015,7 +8015,7 @@
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -8030,13 +8030,13 @@
         <v>195</v>
       </c>
       <c r="F90" t="s">
+        <v>732</v>
+      </c>
+      <c r="G90" t="s">
         <v>733</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>734</v>
-      </c>
-      <c r="H90" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
@@ -8154,7 +8154,7 @@
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B95" t="s">
         <v>1</v>
@@ -8169,15 +8169,15 @@
         <v>216</v>
       </c>
       <c r="F95" t="s">
+        <v>888</v>
+      </c>
+      <c r="G95" t="s">
         <v>889</v>
-      </c>
-      <c r="G95" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
@@ -8192,57 +8192,57 @@
         <v>216</v>
       </c>
       <c r="F96" t="s">
+        <v>891</v>
+      </c>
+      <c r="G96" t="s">
         <v>892</v>
       </c>
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>893</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>894</v>
       </c>
-      <c r="I96" t="s">
+      <c r="J96" t="s">
         <v>895</v>
       </c>
-      <c r="J96" t="s">
+      <c r="K96" t="s">
         <v>896</v>
       </c>
-      <c r="K96" t="s">
+      <c r="L96" t="s">
         <v>897</v>
       </c>
-      <c r="L96" t="s">
+      <c r="M96" t="s">
         <v>898</v>
       </c>
-      <c r="M96" t="s">
+      <c r="N96" t="s">
         <v>899</v>
       </c>
-      <c r="N96" t="s">
+      <c r="O96" t="s">
         <v>900</v>
       </c>
-      <c r="O96" t="s">
+      <c r="P96" t="s">
         <v>901</v>
       </c>
-      <c r="P96" t="s">
+      <c r="Q96" t="s">
         <v>902</v>
       </c>
-      <c r="Q96" t="s">
+      <c r="R96" t="s">
         <v>903</v>
       </c>
-      <c r="R96" t="s">
+      <c r="S96" t="s">
         <v>904</v>
       </c>
-      <c r="S96" t="s">
+      <c r="T96" t="s">
         <v>905</v>
       </c>
-      <c r="T96" t="s">
+      <c r="U96" t="s">
         <v>906</v>
-      </c>
-      <c r="U96" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="97" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
@@ -8257,12 +8257,12 @@
         <v>216</v>
       </c>
       <c r="F97" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="98" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
@@ -8277,36 +8277,36 @@
         <v>216</v>
       </c>
       <c r="F98" t="s">
+        <v>910</v>
+      </c>
+      <c r="G98" t="s">
         <v>911</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>912</v>
       </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>913</v>
       </c>
-      <c r="I98" t="s">
+      <c r="J98" t="s">
         <v>914</v>
       </c>
-      <c r="J98" t="s">
+      <c r="K98" t="s">
         <v>915</v>
       </c>
-      <c r="K98" t="s">
+      <c r="L98" t="s">
         <v>916</v>
       </c>
-      <c r="L98" t="s">
+      <c r="M98" t="s">
         <v>917</v>
       </c>
-      <c r="M98" t="s">
+      <c r="N98" t="s">
         <v>918</v>
-      </c>
-      <c r="N98" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="99" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B99" t="s">
         <v>1</v>
@@ -8318,15 +8318,15 @@
         <v>230</v>
       </c>
       <c r="E99" t="s">
+        <v>920</v>
+      </c>
+      <c r="F99" t="s">
         <v>921</v>
-      </c>
-      <c r="F99" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="100" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B100" t="s">
         <v>1</v>
@@ -8338,30 +8338,30 @@
         <v>230</v>
       </c>
       <c r="E100" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F100" t="s">
+        <v>927</v>
+      </c>
+      <c r="G100" t="s">
         <v>928</v>
       </c>
-      <c r="G100" t="s">
+      <c r="H100" t="s">
         <v>929</v>
       </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
         <v>930</v>
       </c>
-      <c r="I100" t="s">
+      <c r="J100" t="s">
         <v>931</v>
       </c>
-      <c r="J100" t="s">
+      <c r="K100" t="s">
         <v>932</v>
-      </c>
-      <c r="K100" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="101" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
@@ -8373,16 +8373,16 @@
         <v>230</v>
       </c>
       <c r="E101" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F101" t="s">
+        <v>934</v>
+      </c>
+      <c r="G101" t="s">
         <v>935</v>
       </c>
-      <c r="G101" t="s">
+      <c r="H101" t="s">
         <v>936</v>
-      </c>
-      <c r="H101" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="102" spans="1:119" x14ac:dyDescent="0.3">
@@ -8407,30 +8407,30 @@
     </row>
     <row r="103" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>945</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
         <v>946</v>
       </c>
-      <c r="B103" t="s">
-        <v>1</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>947</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>948</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>949</v>
       </c>
-      <c r="F103" t="s">
+      <c r="G103" t="s">
         <v>950</v>
-      </c>
-      <c r="G103" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="104" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B104" t="s">
         <v>1</v>
@@ -8442,39 +8442,39 @@
         <v>29</v>
       </c>
       <c r="E104" t="s">
+        <v>952</v>
+      </c>
+      <c r="F104" t="s">
         <v>953</v>
       </c>
-      <c r="F104" t="s">
+      <c r="G104" t="s">
         <v>954</v>
       </c>
-      <c r="G104" t="s">
+      <c r="H104" t="s">
         <v>955</v>
       </c>
-      <c r="H104" t="s">
+      <c r="I104" t="s">
         <v>956</v>
       </c>
-      <c r="I104" t="s">
+      <c r="J104" t="s">
         <v>957</v>
       </c>
-      <c r="J104" t="s">
+      <c r="K104" t="s">
         <v>958</v>
       </c>
-      <c r="K104" t="s">
+      <c r="L104" t="s">
         <v>959</v>
       </c>
-      <c r="L104" t="s">
+      <c r="M104" t="s">
         <v>960</v>
       </c>
-      <c r="M104" t="s">
+      <c r="N104" t="s">
         <v>961</v>
-      </c>
-      <c r="N104" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="105" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B105" t="s">
         <v>1</v>
@@ -8483,27 +8483,27 @@
         <v>28</v>
       </c>
       <c r="D105" t="s">
+        <v>981</v>
+      </c>
+      <c r="E105" t="s">
         <v>982</v>
       </c>
-      <c r="E105" t="s">
+      <c r="F105" t="s">
         <v>983</v>
       </c>
-      <c r="F105" t="s">
+      <c r="G105" t="s">
         <v>984</v>
       </c>
-      <c r="G105" t="s">
+      <c r="H105" t="s">
         <v>985</v>
       </c>
-      <c r="H105" t="s">
+      <c r="I105" t="s">
         <v>986</v>
-      </c>
-      <c r="I105" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="106" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B106" t="s">
         <v>1</v>
@@ -8512,18 +8512,18 @@
         <v>28</v>
       </c>
       <c r="D106" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E106" t="s">
+        <v>991</v>
+      </c>
+      <c r="F106" t="s">
         <v>992</v>
-      </c>
-      <c r="F106" t="s">
-        <v>993</v>
       </c>
     </row>
     <row r="107" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B107" t="s">
         <v>1</v>
@@ -8532,24 +8532,24 @@
         <v>28</v>
       </c>
       <c r="D107" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E107" t="s">
+        <v>994</v>
+      </c>
+      <c r="F107" t="s">
         <v>995</v>
       </c>
-      <c r="F107" t="s">
+      <c r="G107" t="s">
         <v>996</v>
       </c>
-      <c r="G107" t="s">
+      <c r="H107" t="s">
         <v>997</v>
-      </c>
-      <c r="H107" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="108" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B108" t="s">
         <v>1</v>
@@ -8561,30 +8561,30 @@
         <v>29</v>
       </c>
       <c r="E108" t="s">
+        <v>749</v>
+      </c>
+      <c r="F108" t="s">
         <v>750</v>
       </c>
-      <c r="F108" t="s">
+      <c r="G108" t="s">
         <v>751</v>
       </c>
-      <c r="G108" t="s">
+      <c r="H108" t="s">
         <v>752</v>
       </c>
-      <c r="H108" t="s">
+      <c r="I108" t="s">
         <v>753</v>
       </c>
-      <c r="I108" t="s">
+      <c r="J108" t="s">
         <v>754</v>
       </c>
-      <c r="J108" t="s">
+      <c r="K108" t="s">
         <v>755</v>
-      </c>
-      <c r="K108" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="109" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B109" t="s">
         <v>1</v>
@@ -8596,349 +8596,349 @@
         <v>29</v>
       </c>
       <c r="E109" t="s">
+        <v>758</v>
+      </c>
+      <c r="F109" t="s">
         <v>759</v>
       </c>
-      <c r="F109" t="s">
+      <c r="G109" t="s">
         <v>760</v>
       </c>
-      <c r="G109" t="s">
+      <c r="H109" t="s">
         <v>761</v>
       </c>
-      <c r="H109" t="s">
+      <c r="I109" t="s">
         <v>762</v>
       </c>
-      <c r="I109" t="s">
+      <c r="J109" t="s">
         <v>763</v>
       </c>
-      <c r="J109" t="s">
+      <c r="K109" t="s">
         <v>764</v>
       </c>
-      <c r="K109" t="s">
+      <c r="L109" t="s">
         <v>765</v>
       </c>
-      <c r="L109" t="s">
+      <c r="M109" t="s">
         <v>766</v>
       </c>
-      <c r="M109" t="s">
+      <c r="N109" t="s">
         <v>767</v>
       </c>
-      <c r="N109" t="s">
+      <c r="O109" t="s">
         <v>768</v>
       </c>
-      <c r="O109" t="s">
+      <c r="P109" t="s">
         <v>769</v>
       </c>
-      <c r="P109" t="s">
+      <c r="Q109" t="s">
         <v>770</v>
       </c>
-      <c r="Q109" t="s">
+      <c r="R109" t="s">
         <v>771</v>
       </c>
-      <c r="R109" t="s">
+      <c r="S109" t="s">
         <v>772</v>
       </c>
-      <c r="S109" t="s">
+      <c r="T109" t="s">
         <v>773</v>
       </c>
-      <c r="T109" t="s">
+      <c r="U109" t="s">
         <v>774</v>
       </c>
-      <c r="U109" t="s">
+      <c r="V109" t="s">
         <v>775</v>
       </c>
-      <c r="V109" t="s">
+      <c r="W109" t="s">
         <v>776</v>
       </c>
-      <c r="W109" t="s">
+      <c r="X109" t="s">
         <v>777</v>
       </c>
-      <c r="X109" t="s">
+      <c r="Y109" t="s">
         <v>778</v>
       </c>
-      <c r="Y109" t="s">
+      <c r="Z109" t="s">
         <v>779</v>
       </c>
-      <c r="Z109" t="s">
+      <c r="AA109" t="s">
         <v>780</v>
       </c>
-      <c r="AA109" t="s">
+      <c r="AB109" t="s">
         <v>781</v>
       </c>
-      <c r="AB109" t="s">
+      <c r="AC109" t="s">
         <v>782</v>
       </c>
-      <c r="AC109" t="s">
+      <c r="AD109" t="s">
         <v>783</v>
       </c>
-      <c r="AD109" t="s">
+      <c r="AE109" t="s">
         <v>784</v>
       </c>
-      <c r="AE109" t="s">
+      <c r="AF109" t="s">
         <v>785</v>
       </c>
-      <c r="AF109" t="s">
+      <c r="AG109" t="s">
         <v>786</v>
       </c>
-      <c r="AG109" t="s">
+      <c r="AH109" t="s">
         <v>787</v>
       </c>
-      <c r="AH109" t="s">
+      <c r="AI109" t="s">
         <v>788</v>
       </c>
-      <c r="AI109" t="s">
+      <c r="AJ109" t="s">
         <v>789</v>
       </c>
-      <c r="AJ109" t="s">
+      <c r="AK109" t="s">
         <v>790</v>
       </c>
-      <c r="AK109" t="s">
+      <c r="AL109" t="s">
         <v>791</v>
       </c>
-      <c r="AL109" t="s">
+      <c r="AM109" t="s">
         <v>792</v>
       </c>
-      <c r="AM109" t="s">
+      <c r="AN109" t="s">
         <v>793</v>
       </c>
-      <c r="AN109" t="s">
+      <c r="AO109" t="s">
         <v>794</v>
       </c>
-      <c r="AO109" t="s">
+      <c r="AP109" t="s">
         <v>795</v>
       </c>
-      <c r="AP109" t="s">
+      <c r="AQ109" t="s">
         <v>796</v>
       </c>
-      <c r="AQ109" t="s">
+      <c r="AR109" t="s">
         <v>797</v>
       </c>
-      <c r="AR109" t="s">
+      <c r="AS109" t="s">
         <v>798</v>
       </c>
-      <c r="AS109" t="s">
+      <c r="AT109" t="s">
         <v>799</v>
       </c>
-      <c r="AT109" t="s">
+      <c r="AU109" t="s">
         <v>800</v>
       </c>
-      <c r="AU109" t="s">
+      <c r="AV109" t="s">
         <v>801</v>
       </c>
-      <c r="AV109" t="s">
+      <c r="AW109" t="s">
         <v>802</v>
       </c>
-      <c r="AW109" t="s">
+      <c r="AX109" t="s">
         <v>803</v>
       </c>
-      <c r="AX109" t="s">
+      <c r="AY109" t="s">
         <v>804</v>
       </c>
-      <c r="AY109" t="s">
+      <c r="AZ109" t="s">
         <v>805</v>
       </c>
-      <c r="AZ109" t="s">
+      <c r="BA109" t="s">
         <v>806</v>
       </c>
-      <c r="BA109" t="s">
+      <c r="BB109" t="s">
         <v>807</v>
       </c>
-      <c r="BB109" t="s">
+      <c r="BC109" t="s">
         <v>808</v>
       </c>
-      <c r="BC109" t="s">
+      <c r="BD109" t="s">
         <v>809</v>
       </c>
-      <c r="BD109" t="s">
+      <c r="BE109" t="s">
         <v>810</v>
       </c>
-      <c r="BE109" t="s">
+      <c r="BF109" t="s">
         <v>811</v>
       </c>
-      <c r="BF109" t="s">
+      <c r="BG109" t="s">
         <v>812</v>
       </c>
-      <c r="BG109" t="s">
+      <c r="BH109" t="s">
         <v>813</v>
       </c>
-      <c r="BH109" t="s">
+      <c r="BI109" t="s">
         <v>814</v>
       </c>
-      <c r="BI109" t="s">
+      <c r="BJ109" t="s">
         <v>815</v>
       </c>
-      <c r="BJ109" t="s">
+      <c r="BK109" t="s">
         <v>816</v>
       </c>
-      <c r="BK109" t="s">
+      <c r="BL109" t="s">
         <v>817</v>
       </c>
-      <c r="BL109" t="s">
+      <c r="BM109" t="s">
         <v>818</v>
       </c>
-      <c r="BM109" t="s">
+      <c r="BN109" t="s">
         <v>819</v>
       </c>
-      <c r="BN109" t="s">
+      <c r="BO109" t="s">
         <v>820</v>
       </c>
-      <c r="BO109" t="s">
+      <c r="BP109" t="s">
         <v>821</v>
       </c>
-      <c r="BP109" t="s">
+      <c r="BQ109" t="s">
         <v>822</v>
       </c>
-      <c r="BQ109" t="s">
+      <c r="BR109" t="s">
         <v>823</v>
       </c>
-      <c r="BR109" t="s">
+      <c r="BS109" t="s">
         <v>824</v>
       </c>
-      <c r="BS109" t="s">
+      <c r="BT109" t="s">
         <v>825</v>
       </c>
-      <c r="BT109" t="s">
+      <c r="BU109" t="s">
         <v>826</v>
       </c>
-      <c r="BU109" t="s">
+      <c r="BV109" t="s">
         <v>827</v>
       </c>
-      <c r="BV109" t="s">
+      <c r="BW109" t="s">
         <v>828</v>
       </c>
-      <c r="BW109" t="s">
+      <c r="BX109" t="s">
         <v>829</v>
       </c>
-      <c r="BX109" t="s">
+      <c r="BY109" t="s">
         <v>830</v>
       </c>
-      <c r="BY109" t="s">
+      <c r="BZ109" t="s">
         <v>831</v>
       </c>
-      <c r="BZ109" t="s">
+      <c r="CA109" t="s">
         <v>832</v>
       </c>
-      <c r="CA109" t="s">
+      <c r="CB109" t="s">
         <v>833</v>
       </c>
-      <c r="CB109" t="s">
+      <c r="CC109" t="s">
         <v>834</v>
       </c>
-      <c r="CC109" t="s">
+      <c r="CD109" t="s">
         <v>835</v>
       </c>
-      <c r="CD109" t="s">
+      <c r="CE109" t="s">
         <v>836</v>
       </c>
-      <c r="CE109" t="s">
+      <c r="CF109" t="s">
         <v>837</v>
       </c>
-      <c r="CF109" t="s">
+      <c r="CG109" t="s">
         <v>838</v>
       </c>
-      <c r="CG109" t="s">
+      <c r="CH109" t="s">
         <v>839</v>
       </c>
-      <c r="CH109" t="s">
+      <c r="CI109" t="s">
         <v>840</v>
       </c>
-      <c r="CI109" t="s">
+      <c r="CJ109" t="s">
         <v>841</v>
       </c>
-      <c r="CJ109" t="s">
+      <c r="CK109" t="s">
         <v>842</v>
       </c>
-      <c r="CK109" t="s">
+      <c r="CL109" t="s">
         <v>843</v>
       </c>
-      <c r="CL109" t="s">
+      <c r="CM109" t="s">
         <v>844</v>
       </c>
-      <c r="CM109" t="s">
+      <c r="CN109" t="s">
         <v>845</v>
       </c>
-      <c r="CN109" t="s">
+      <c r="CO109" t="s">
         <v>846</v>
       </c>
-      <c r="CO109" t="s">
+      <c r="CP109" t="s">
         <v>847</v>
       </c>
-      <c r="CP109" t="s">
+      <c r="CQ109" t="s">
         <v>848</v>
       </c>
-      <c r="CQ109" t="s">
+      <c r="CR109" t="s">
         <v>849</v>
       </c>
-      <c r="CR109" t="s">
+      <c r="CS109" t="s">
         <v>850</v>
       </c>
-      <c r="CS109" t="s">
+      <c r="CT109" t="s">
         <v>851</v>
       </c>
-      <c r="CT109" t="s">
+      <c r="CU109" t="s">
         <v>852</v>
       </c>
-      <c r="CU109" t="s">
+      <c r="CV109" t="s">
         <v>853</v>
       </c>
-      <c r="CV109" t="s">
+      <c r="CW109" t="s">
         <v>854</v>
       </c>
-      <c r="CW109" t="s">
+      <c r="CX109" t="s">
         <v>855</v>
       </c>
-      <c r="CX109" t="s">
+      <c r="CY109" t="s">
         <v>856</v>
       </c>
-      <c r="CY109" t="s">
+      <c r="CZ109" t="s">
         <v>857</v>
       </c>
-      <c r="CZ109" t="s">
+      <c r="DA109" t="s">
         <v>858</v>
       </c>
-      <c r="DA109" t="s">
+      <c r="DB109" t="s">
         <v>859</v>
       </c>
-      <c r="DB109" t="s">
+      <c r="DC109" t="s">
         <v>860</v>
       </c>
-      <c r="DC109" t="s">
+      <c r="DD109" t="s">
         <v>861</v>
       </c>
-      <c r="DD109" t="s">
+      <c r="DE109" t="s">
         <v>862</v>
       </c>
-      <c r="DE109" t="s">
+      <c r="DF109" t="s">
         <v>863</v>
       </c>
-      <c r="DF109" t="s">
+      <c r="DG109" t="s">
         <v>864</v>
       </c>
-      <c r="DG109" t="s">
+      <c r="DH109" t="s">
         <v>865</v>
       </c>
-      <c r="DH109" t="s">
+      <c r="DI109" t="s">
         <v>866</v>
       </c>
-      <c r="DI109" t="s">
+      <c r="DJ109" t="s">
         <v>867</v>
       </c>
-      <c r="DJ109" t="s">
+      <c r="DK109" t="s">
         <v>868</v>
       </c>
-      <c r="DK109" t="s">
+      <c r="DL109" t="s">
         <v>869</v>
       </c>
-      <c r="DL109" t="s">
+      <c r="DM109" t="s">
         <v>870</v>
       </c>
-      <c r="DM109" t="s">
+      <c r="DN109" t="s">
         <v>871</v>
       </c>
-      <c r="DN109" t="s">
+      <c r="DO109" t="s">
         <v>872</v>
-      </c>
-      <c r="DO109" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="110" spans="1:119" x14ac:dyDescent="0.3">
@@ -8983,7 +8983,7 @@
     </row>
     <row r="112" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B112" t="s">
         <v>1</v>
@@ -8998,12 +8998,12 @@
         <v>4</v>
       </c>
       <c r="F112" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B113" t="s">
         <v>1</v>
@@ -9018,16 +9018,16 @@
         <v>4</v>
       </c>
       <c r="F113" t="s">
+        <v>1001</v>
+      </c>
+      <c r="G113" t="s">
         <v>1002</v>
       </c>
-      <c r="G113" t="s">
+      <c r="H113" t="s">
         <v>1003</v>
       </c>
-      <c r="H113" t="s">
+      <c r="I113" t="s">
         <v>1004</v>
-      </c>
-      <c r="I113" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.3">
@@ -9052,7 +9052,7 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B115" t="s">
         <v>1</v>
@@ -9067,10 +9067,10 @@
         <v>4</v>
       </c>
       <c r="F115" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G115" t="s">
         <v>1007</v>
-      </c>
-      <c r="G115" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
@@ -9095,7 +9095,7 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B117" t="s">
         <v>1</v>
@@ -9104,24 +9104,24 @@
         <v>2</v>
       </c>
       <c r="D117" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E117" t="s">
         <v>1011</v>
       </c>
-      <c r="E117" t="s">
+      <c r="F117" t="s">
         <v>1012</v>
       </c>
-      <c r="F117" t="s">
+      <c r="G117" t="s">
         <v>1013</v>
       </c>
-      <c r="G117" t="s">
+      <c r="H117" t="s">
         <v>1014</v>
-      </c>
-      <c r="H117" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B118" t="s">
         <v>1</v>
@@ -9130,18 +9130,18 @@
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E118" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F118" t="s">
         <v>1020</v>
-      </c>
-      <c r="F118" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B119" t="s">
         <v>1</v>
@@ -9150,13 +9150,13 @@
         <v>2</v>
       </c>
       <c r="D119" t="s">
+        <v>740</v>
+      </c>
+      <c r="E119" t="s">
         <v>741</v>
       </c>
-      <c r="E119" t="s">
+      <c r="F119" t="s">
         <v>742</v>
-      </c>
-      <c r="F119" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.3">
@@ -9214,7 +9214,7 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B121" t="s">
         <v>122</v>
@@ -9223,13 +9223,13 @@
         <v>123</v>
       </c>
       <c r="D121" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E121" t="s">
         <v>1042</v>
       </c>
-      <c r="E121" t="s">
+      <c r="F121" t="s">
         <v>1043</v>
-      </c>
-      <c r="F121" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.3">
@@ -9490,7 +9490,7 @@
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B130" t="s">
         <v>1</v>
@@ -9502,13 +9502,13 @@
         <v>724</v>
       </c>
       <c r="E130" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F130" t="s">
         <v>1046</v>
       </c>
-      <c r="F130" t="s">
+      <c r="G130" t="s">
         <v>1047</v>
-      </c>
-      <c r="G130" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.3">
@@ -9528,12 +9528,12 @@
         <v>725</v>
       </c>
       <c r="F131" t="s">
-        <v>726</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B132" t="s">
         <v>1</v>
@@ -9548,7 +9548,7 @@
         <v>9</v>
       </c>
       <c r="F132" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.3">
@@ -9599,7 +9599,7 @@
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B135" t="s">
         <v>1</v>
@@ -9614,18 +9614,18 @@
         <v>9</v>
       </c>
       <c r="F135" t="s">
+        <v>1062</v>
+      </c>
+      <c r="G135" t="s">
         <v>1063</v>
       </c>
-      <c r="G135" t="s">
+      <c r="H135" t="s">
         <v>1064</v>
-      </c>
-      <c r="H135" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B136" t="s">
         <v>1</v>
@@ -9640,15 +9640,15 @@
         <v>9</v>
       </c>
       <c r="F136" t="s">
+        <v>1067</v>
+      </c>
+      <c r="G136" t="s">
         <v>1068</v>
-      </c>
-      <c r="G136" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B137" t="s">
         <v>1</v>
@@ -9663,15 +9663,15 @@
         <v>9</v>
       </c>
       <c r="F137" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G137" t="s">
         <v>1071</v>
-      </c>
-      <c r="G137" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B138" t="s">
         <v>1</v>
@@ -9686,28 +9686,28 @@
         <v>9</v>
       </c>
       <c r="F138" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G138" t="s">
         <v>1074</v>
       </c>
-      <c r="G138" t="s">
+      <c r="H138" t="s">
         <v>1075</v>
       </c>
-      <c r="H138" t="s">
+      <c r="I138" t="s">
         <v>1076</v>
       </c>
-      <c r="I138" t="s">
+      <c r="J138" t="s">
         <v>1077</v>
       </c>
-      <c r="J138" t="s">
+      <c r="K138" t="s">
         <v>1078</v>
       </c>
-      <c r="K138" t="s">
+      <c r="L138" t="s">
         <v>1079</v>
       </c>
-      <c r="L138" t="s">
+      <c r="M138" t="s">
         <v>1080</v>
-      </c>
-      <c r="M138" t="s">
-        <v>1081</v>
       </c>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.3">
@@ -9761,7 +9761,7 @@
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B141" t="s">
         <v>1</v>
@@ -9784,7 +9784,7 @@
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B142" t="s">
         <v>1</v>
@@ -9807,7 +9807,7 @@
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B143" t="s">
         <v>1</v>
@@ -9830,7 +9830,7 @@
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B144" t="s">
         <v>1</v>
@@ -9845,7 +9845,7 @@
         <v>9</v>
       </c>
       <c r="F144" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G144" t="s">
         <v>698</v>
@@ -9853,7 +9853,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B145" t="s">
         <v>1</v>
@@ -9876,7 +9876,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B146" t="s">
         <v>1</v>
@@ -9899,7 +9899,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B147" t="s">
         <v>1</v>
@@ -9919,7 +9919,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B148" t="s">
         <v>1</v>
@@ -9939,7 +9939,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B149" t="s">
         <v>1</v>
@@ -9954,7 +9954,7 @@
         <v>9</v>
       </c>
       <c r="F149" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G149" t="s">
         <v>698</v>
@@ -9962,7 +9962,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B150" t="s">
         <v>1</v>
@@ -10117,7 +10117,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B157" t="s">
         <v>1</v>
@@ -10160,7 +10160,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B159" t="s">
         <v>1</v>
@@ -10226,7 +10226,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B162" t="s">
         <v>1</v>
@@ -10241,15 +10241,15 @@
         <v>231</v>
       </c>
       <c r="F162" t="s">
+        <v>879</v>
+      </c>
+      <c r="G162" t="s">
         <v>880</v>
-      </c>
-      <c r="G162" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B163" t="s">
         <v>1</v>
@@ -10272,7 +10272,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B164" t="s">
         <v>1</v>
@@ -10295,7 +10295,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B165" t="s">
         <v>1</v>
@@ -10318,7 +10318,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B166" t="s">
         <v>1</v>
@@ -10333,12 +10333,12 @@
         <v>231</v>
       </c>
       <c r="F166" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B167" t="s">
         <v>1</v>
@@ -10361,7 +10361,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B168" t="s">
         <v>1</v>
@@ -10376,15 +10376,15 @@
         <v>231</v>
       </c>
       <c r="F168" t="s">
+        <v>879</v>
+      </c>
+      <c r="G168" t="s">
         <v>880</v>
-      </c>
-      <c r="G168" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B169" t="s">
         <v>1</v>
@@ -10399,12 +10399,12 @@
         <v>231</v>
       </c>
       <c r="F169" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B170" t="s">
         <v>1</v>
@@ -10427,7 +10427,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B171" t="s">
         <v>1</v>
@@ -10442,15 +10442,15 @@
         <v>231</v>
       </c>
       <c r="F171" t="s">
+        <v>879</v>
+      </c>
+      <c r="G171" t="s">
         <v>880</v>
-      </c>
-      <c r="G171" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B172" t="s">
         <v>1</v>
@@ -10465,15 +10465,15 @@
         <v>231</v>
       </c>
       <c r="F172" t="s">
+        <v>879</v>
+      </c>
+      <c r="G172" t="s">
         <v>880</v>
-      </c>
-      <c r="G172" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B173" t="s">
         <v>1</v>
@@ -10542,7 +10542,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B176" t="s">
         <v>1</v>
@@ -10588,7 +10588,7 @@
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B178" t="s">
         <v>1</v>
@@ -10611,7 +10611,7 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B179" t="s">
         <v>1</v>
@@ -10634,7 +10634,7 @@
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B180" t="s">
         <v>1</v>
@@ -10649,15 +10649,15 @@
         <v>231</v>
       </c>
       <c r="F180" t="s">
+        <v>879</v>
+      </c>
+      <c r="G180" t="s">
         <v>880</v>
-      </c>
-      <c r="G180" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
@@ -10669,15 +10669,15 @@
         <v>8</v>
       </c>
       <c r="E181" t="s">
+        <v>942</v>
+      </c>
+      <c r="F181" t="s">
         <v>943</v>
-      </c>
-      <c r="F181" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B182" t="s">
         <v>1</v>
@@ -10689,7 +10689,7 @@
         <v>8</v>
       </c>
       <c r="E182" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F182" t="s">
         <v>239</v>
@@ -10700,7 +10700,7 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B183" t="s">
         <v>1</v>
@@ -10712,18 +10712,18 @@
         <v>256</v>
       </c>
       <c r="E183" t="s">
+        <v>923</v>
+      </c>
+      <c r="F183" t="s">
         <v>924</v>
       </c>
-      <c r="F183" t="s">
+      <c r="G183" t="s">
         <v>925</v>
-      </c>
-      <c r="G183" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B184" t="s">
         <v>1</v>
@@ -10735,36 +10735,36 @@
         <v>256</v>
       </c>
       <c r="E184" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F184" t="s">
         <v>1209</v>
       </c>
-      <c r="F184" t="s">
+      <c r="G184" t="s">
         <v>1210</v>
       </c>
-      <c r="G184" t="s">
+      <c r="H184" t="s">
         <v>1211</v>
       </c>
-      <c r="H184" t="s">
+      <c r="I184" t="s">
         <v>1212</v>
       </c>
-      <c r="I184" t="s">
+      <c r="J184" t="s">
         <v>1213</v>
       </c>
-      <c r="J184" t="s">
+      <c r="K184" t="s">
         <v>1214</v>
       </c>
-      <c r="K184" t="s">
+      <c r="L184" t="s">
         <v>1215</v>
       </c>
-      <c r="L184" t="s">
+      <c r="M184" t="s">
         <v>1216</v>
-      </c>
-      <c r="M184" t="s">
-        <v>1217</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="B185" t="s">
         <v>1</v>
@@ -10776,16 +10776,16 @@
         <v>256</v>
       </c>
       <c r="E185" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F185" t="s">
         <v>1417</v>
       </c>
-      <c r="F185" t="s">
+      <c r="G185" t="s">
         <v>1418</v>
       </c>
-      <c r="G185" t="s">
+      <c r="H185" t="s">
         <v>1419</v>
-      </c>
-      <c r="H185" t="s">
-        <v>1420</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.3">
@@ -10828,7 +10828,7 @@
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B187" t="s">
         <v>1</v>
@@ -10840,27 +10840,27 @@
         <v>256</v>
       </c>
       <c r="E187" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F187" t="s">
         <v>1219</v>
       </c>
-      <c r="F187" t="s">
+      <c r="G187" t="s">
         <v>1220</v>
       </c>
-      <c r="G187" t="s">
+      <c r="H187" t="s">
         <v>1221</v>
       </c>
-      <c r="H187" t="s">
+      <c r="I187" t="s">
         <v>1222</v>
       </c>
-      <c r="I187" t="s">
+      <c r="J187" t="s">
         <v>1223</v>
-      </c>
-      <c r="J187" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B188" t="s">
         <v>1</v>
@@ -10872,15 +10872,15 @@
         <v>3</v>
       </c>
       <c r="E188" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F188" t="s">
         <v>1226</v>
-      </c>
-      <c r="F188" t="s">
-        <v>1227</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B189" t="s">
         <v>1</v>
@@ -10892,24 +10892,24 @@
         <v>3</v>
       </c>
       <c r="E189" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F189" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G189" t="s">
         <v>1226</v>
       </c>
-      <c r="F189" t="s">
+      <c r="H189" t="s">
         <v>1229</v>
       </c>
-      <c r="G189" t="s">
-        <v>1227</v>
-      </c>
-      <c r="H189" t="s">
+      <c r="I189" t="s">
         <v>1230</v>
-      </c>
-      <c r="I189" t="s">
-        <v>1231</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B190" t="s">
         <v>122</v>
@@ -10918,18 +10918,18 @@
         <v>123</v>
       </c>
       <c r="D190" t="s">
+        <v>938</v>
+      </c>
+      <c r="E190" t="s">
         <v>939</v>
       </c>
-      <c r="E190" t="s">
+      <c r="F190" t="s">
         <v>940</v>
-      </c>
-      <c r="F190" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B191" t="s">
         <v>1</v>
@@ -10938,21 +10938,21 @@
         <v>2</v>
       </c>
       <c r="D191" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E191" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F191" t="s">
         <v>1204</v>
       </c>
-      <c r="F191" t="s">
+      <c r="G191" t="s">
         <v>1205</v>
-      </c>
-      <c r="G191" t="s">
-        <v>1206</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B192" t="s">
         <v>1</v>
@@ -10961,21 +10961,21 @@
         <v>2</v>
       </c>
       <c r="D192" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E192" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F192" t="s">
         <v>1200</v>
       </c>
-      <c r="F192" t="s">
+      <c r="G192" t="s">
         <v>1201</v>
-      </c>
-      <c r="G192" t="s">
-        <v>1202</v>
       </c>
     </row>
     <row r="193" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B193" t="s">
         <v>1</v>
@@ -10987,294 +10987,294 @@
         <v>370</v>
       </c>
       <c r="E193" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F193" t="s">
         <v>1094</v>
       </c>
-      <c r="F193" t="s">
+      <c r="G193" t="s">
         <v>1095</v>
       </c>
-      <c r="G193" t="s">
+      <c r="H193" t="s">
         <v>1096</v>
       </c>
-      <c r="H193" t="s">
+      <c r="I193" t="s">
         <v>1097</v>
       </c>
-      <c r="I193" t="s">
+      <c r="J193" t="s">
         <v>1098</v>
       </c>
-      <c r="J193" t="s">
+      <c r="K193" t="s">
         <v>1099</v>
       </c>
-      <c r="K193" t="s">
+      <c r="L193" t="s">
         <v>1100</v>
       </c>
-      <c r="L193" t="s">
+      <c r="M193" t="s">
         <v>1101</v>
       </c>
-      <c r="M193" t="s">
+      <c r="N193" t="s">
         <v>1102</v>
       </c>
-      <c r="N193" t="s">
+      <c r="O193" t="s">
         <v>1103</v>
       </c>
-      <c r="O193" t="s">
+      <c r="P193" t="s">
         <v>1104</v>
       </c>
-      <c r="P193" t="s">
+      <c r="Q193" t="s">
         <v>1105</v>
       </c>
-      <c r="Q193" t="s">
+      <c r="R193" t="s">
         <v>1106</v>
       </c>
-      <c r="R193" t="s">
+      <c r="S193" t="s">
         <v>1107</v>
       </c>
-      <c r="S193" t="s">
+      <c r="T193" t="s">
         <v>1108</v>
       </c>
-      <c r="T193" t="s">
+      <c r="U193" t="s">
         <v>1109</v>
       </c>
-      <c r="U193" t="s">
+      <c r="V193" t="s">
         <v>1110</v>
       </c>
-      <c r="V193" t="s">
+      <c r="W193" t="s">
         <v>1111</v>
       </c>
-      <c r="W193" t="s">
+      <c r="X193" t="s">
         <v>1112</v>
       </c>
-      <c r="X193" t="s">
+      <c r="Y193" t="s">
         <v>1113</v>
       </c>
-      <c r="Y193" t="s">
+      <c r="Z193" t="s">
         <v>1114</v>
       </c>
-      <c r="Z193" t="s">
+      <c r="AA193" t="s">
         <v>1115</v>
       </c>
-      <c r="AA193" t="s">
+      <c r="AB193" t="s">
         <v>1116</v>
       </c>
-      <c r="AB193" t="s">
+      <c r="AC193" t="s">
         <v>1117</v>
       </c>
-      <c r="AC193" t="s">
+      <c r="AD193" t="s">
         <v>1118</v>
       </c>
-      <c r="AD193" t="s">
+      <c r="AE193" t="s">
         <v>1119</v>
       </c>
-      <c r="AE193" t="s">
+      <c r="AF193" t="s">
         <v>1120</v>
       </c>
-      <c r="AF193" t="s">
+      <c r="AG193" t="s">
         <v>1121</v>
       </c>
-      <c r="AG193" t="s">
+      <c r="AH193" t="s">
         <v>1122</v>
       </c>
-      <c r="AH193" t="s">
+      <c r="AI193" t="s">
         <v>1123</v>
       </c>
-      <c r="AI193" t="s">
+      <c r="AJ193" t="s">
         <v>1124</v>
       </c>
-      <c r="AJ193" t="s">
+      <c r="AK193" t="s">
         <v>1125</v>
       </c>
-      <c r="AK193" t="s">
+      <c r="AL193" t="s">
         <v>1126</v>
       </c>
-      <c r="AL193" t="s">
+      <c r="AM193" t="s">
         <v>1127</v>
       </c>
-      <c r="AM193" t="s">
+      <c r="AN193" t="s">
         <v>1128</v>
       </c>
-      <c r="AN193" t="s">
+      <c r="AO193" t="s">
         <v>1129</v>
       </c>
-      <c r="AO193" t="s">
+      <c r="AP193" t="s">
         <v>1130</v>
       </c>
-      <c r="AP193" t="s">
+      <c r="AQ193" t="s">
         <v>1131</v>
       </c>
-      <c r="AQ193" t="s">
+      <c r="AR193" t="s">
         <v>1132</v>
       </c>
-      <c r="AR193" t="s">
+      <c r="AS193" t="s">
         <v>1133</v>
       </c>
-      <c r="AS193" t="s">
+      <c r="AT193" t="s">
         <v>1134</v>
       </c>
-      <c r="AT193" t="s">
+      <c r="AU193" t="s">
         <v>1135</v>
       </c>
-      <c r="AU193" t="s">
+      <c r="AV193" t="s">
         <v>1136</v>
       </c>
-      <c r="AV193" t="s">
+      <c r="AW193" t="s">
         <v>1137</v>
       </c>
-      <c r="AW193" t="s">
+      <c r="AX193" t="s">
         <v>1138</v>
       </c>
-      <c r="AX193" t="s">
+      <c r="AY193" t="s">
         <v>1139</v>
       </c>
-      <c r="AY193" t="s">
+      <c r="AZ193" t="s">
         <v>1140</v>
       </c>
-      <c r="AZ193" t="s">
+      <c r="BA193" t="s">
         <v>1141</v>
       </c>
-      <c r="BA193" t="s">
+      <c r="BB193" t="s">
         <v>1142</v>
       </c>
-      <c r="BB193" t="s">
+      <c r="BC193" t="s">
         <v>1143</v>
       </c>
-      <c r="BC193" t="s">
+      <c r="BD193" t="s">
         <v>1144</v>
       </c>
-      <c r="BD193" t="s">
+      <c r="BE193" t="s">
         <v>1145</v>
       </c>
-      <c r="BE193" t="s">
+      <c r="BF193" t="s">
         <v>1146</v>
       </c>
-      <c r="BF193" t="s">
+      <c r="BG193" t="s">
         <v>1147</v>
       </c>
-      <c r="BG193" t="s">
+      <c r="BH193" t="s">
         <v>1148</v>
       </c>
-      <c r="BH193" t="s">
+      <c r="BI193" t="s">
         <v>1149</v>
       </c>
-      <c r="BI193" t="s">
+      <c r="BJ193" t="s">
         <v>1150</v>
       </c>
-      <c r="BJ193" t="s">
+      <c r="BK193" t="s">
         <v>1151</v>
       </c>
-      <c r="BK193" t="s">
+      <c r="BL193" t="s">
         <v>1152</v>
       </c>
-      <c r="BL193" t="s">
+      <c r="BM193" t="s">
         <v>1153</v>
       </c>
-      <c r="BM193" t="s">
+      <c r="BN193" t="s">
         <v>1154</v>
       </c>
-      <c r="BN193" t="s">
+      <c r="BO193" t="s">
         <v>1155</v>
       </c>
-      <c r="BO193" t="s">
+      <c r="BP193" t="s">
         <v>1156</v>
       </c>
-      <c r="BP193" t="s">
+      <c r="BQ193" t="s">
         <v>1157</v>
       </c>
-      <c r="BQ193" t="s">
+      <c r="BR193" t="s">
         <v>1158</v>
       </c>
-      <c r="BR193" t="s">
+      <c r="BS193" t="s">
         <v>1159</v>
       </c>
-      <c r="BS193" t="s">
+      <c r="BT193" t="s">
         <v>1160</v>
       </c>
-      <c r="BT193" t="s">
+      <c r="BU193" t="s">
         <v>1161</v>
       </c>
-      <c r="BU193" t="s">
+      <c r="BV193" t="s">
         <v>1162</v>
       </c>
-      <c r="BV193" t="s">
+      <c r="BW193" t="s">
         <v>1163</v>
       </c>
-      <c r="BW193" t="s">
+      <c r="BX193" t="s">
         <v>1164</v>
       </c>
-      <c r="BX193" t="s">
+      <c r="BY193" t="s">
         <v>1165</v>
       </c>
-      <c r="BY193" t="s">
+      <c r="BZ193" t="s">
         <v>1166</v>
       </c>
-      <c r="BZ193" t="s">
+      <c r="CA193" t="s">
         <v>1167</v>
       </c>
-      <c r="CA193" t="s">
+      <c r="CB193" t="s">
         <v>1168</v>
       </c>
-      <c r="CB193" t="s">
+      <c r="CC193" t="s">
         <v>1169</v>
       </c>
-      <c r="CC193" t="s">
+      <c r="CD193" t="s">
         <v>1170</v>
       </c>
-      <c r="CD193" t="s">
+      <c r="CE193" t="s">
         <v>1171</v>
       </c>
-      <c r="CE193" t="s">
+      <c r="CF193" t="s">
         <v>1172</v>
       </c>
-      <c r="CF193" t="s">
+      <c r="CG193" t="s">
         <v>1173</v>
       </c>
-      <c r="CG193" t="s">
+      <c r="CH193" t="s">
         <v>1174</v>
       </c>
-      <c r="CH193" t="s">
+      <c r="CI193" t="s">
         <v>1175</v>
       </c>
-      <c r="CI193" t="s">
+      <c r="CJ193" t="s">
         <v>1176</v>
       </c>
-      <c r="CJ193" t="s">
+      <c r="CK193" t="s">
         <v>1177</v>
       </c>
-      <c r="CK193" t="s">
+      <c r="CL193" t="s">
         <v>1178</v>
       </c>
-      <c r="CL193" t="s">
+      <c r="CM193" t="s">
         <v>1179</v>
       </c>
-      <c r="CM193" t="s">
+      <c r="CN193" t="s">
         <v>1180</v>
       </c>
-      <c r="CN193" t="s">
+      <c r="CO193" t="s">
         <v>1181</v>
       </c>
-      <c r="CO193" t="s">
+      <c r="CP193" t="s">
         <v>1182</v>
       </c>
-      <c r="CP193" t="s">
+      <c r="CQ193" t="s">
         <v>1183</v>
       </c>
-      <c r="CQ193" t="s">
+      <c r="CR193" t="s">
         <v>1184</v>
       </c>
-      <c r="CR193" t="s">
+      <c r="CS193" t="s">
         <v>1185</v>
       </c>
-      <c r="CS193" t="s">
+      <c r="CT193" t="s">
         <v>1186</v>
       </c>
-      <c r="CT193" t="s">
+      <c r="CU193" t="s">
         <v>1187</v>
-      </c>
-      <c r="CU193" t="s">
-        <v>1188</v>
       </c>
     </row>
     <row r="194" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B194" t="s">
         <v>1</v>
@@ -11283,27 +11283,27 @@
         <v>16</v>
       </c>
       <c r="D194" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E194" t="s">
         <v>1233</v>
       </c>
-      <c r="E194" t="s">
+      <c r="F194" t="s">
         <v>1234</v>
       </c>
-      <c r="F194" t="s">
+      <c r="G194" t="s">
         <v>1235</v>
       </c>
-      <c r="G194" t="s">
+      <c r="H194" t="s">
         <v>1236</v>
       </c>
-      <c r="H194" t="s">
+      <c r="I194" t="s">
         <v>1237</v>
-      </c>
-      <c r="I194" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="195" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B195" t="s">
         <v>1</v>
@@ -11315,10 +11315,10 @@
         <v>88</v>
       </c>
       <c r="E195" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F195" t="s">
         <v>1240</v>
-      </c>
-      <c r="F195" t="s">
-        <v>1241</v>
       </c>
     </row>
     <row r="196" spans="1:99" x14ac:dyDescent="0.3">
@@ -11399,7 +11399,7 @@
     </row>
     <row r="198" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B198" t="s">
         <v>1</v>
@@ -11411,15 +11411,15 @@
         <v>394</v>
       </c>
       <c r="E198" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F198" t="s">
         <v>1243</v>
-      </c>
-      <c r="F198" t="s">
-        <v>1244</v>
       </c>
     </row>
     <row r="199" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B199" t="s">
         <v>1</v>
@@ -11434,216 +11434,216 @@
         <v>148</v>
       </c>
       <c r="F199" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G199" t="s">
         <v>1246</v>
       </c>
-      <c r="G199" t="s">
+      <c r="H199" t="s">
         <v>1247</v>
       </c>
-      <c r="H199" t="s">
+      <c r="I199" t="s">
         <v>1248</v>
       </c>
-      <c r="I199" t="s">
+      <c r="J199" t="s">
         <v>1249</v>
       </c>
-      <c r="J199" t="s">
+      <c r="K199" t="s">
         <v>1250</v>
       </c>
-      <c r="K199" t="s">
+      <c r="L199" t="s">
         <v>1251</v>
       </c>
-      <c r="L199" t="s">
+      <c r="M199" t="s">
         <v>1252</v>
       </c>
-      <c r="M199" t="s">
+      <c r="N199" t="s">
         <v>1253</v>
       </c>
-      <c r="N199" t="s">
+      <c r="O199" t="s">
         <v>1254</v>
       </c>
-      <c r="O199" t="s">
+      <c r="P199" t="s">
         <v>1255</v>
       </c>
-      <c r="P199" t="s">
+      <c r="Q199" t="s">
         <v>1256</v>
       </c>
-      <c r="Q199" t="s">
+      <c r="R199" t="s">
         <v>1257</v>
       </c>
-      <c r="R199" t="s">
+      <c r="S199" t="s">
         <v>1258</v>
       </c>
-      <c r="S199" t="s">
+      <c r="T199" t="s">
         <v>1259</v>
       </c>
-      <c r="T199" t="s">
+      <c r="U199" t="s">
         <v>1260</v>
       </c>
-      <c r="U199" t="s">
+      <c r="V199" t="s">
         <v>1261</v>
       </c>
-      <c r="V199" t="s">
+      <c r="W199" t="s">
         <v>1262</v>
       </c>
-      <c r="W199" t="s">
+      <c r="X199" t="s">
         <v>1263</v>
       </c>
-      <c r="X199" t="s">
+      <c r="Y199" t="s">
         <v>1264</v>
       </c>
-      <c r="Y199" t="s">
+      <c r="Z199" t="s">
+        <v>1420</v>
+      </c>
+      <c r="AA199" t="s">
+        <v>1421</v>
+      </c>
+      <c r="AB199" t="s">
+        <v>1422</v>
+      </c>
+      <c r="AC199" t="s">
         <v>1265</v>
       </c>
-      <c r="Z199" t="s">
-        <v>1421</v>
-      </c>
-      <c r="AA199" t="s">
-        <v>1422</v>
-      </c>
-      <c r="AB199" t="s">
+      <c r="AD199" t="s">
+        <v>1266</v>
+      </c>
+      <c r="AE199" t="s">
+        <v>1267</v>
+      </c>
+      <c r="AF199" t="s">
+        <v>1268</v>
+      </c>
+      <c r="AG199" t="s">
+        <v>1269</v>
+      </c>
+      <c r="AH199" t="s">
         <v>1423</v>
       </c>
-      <c r="AC199" t="s">
-        <v>1266</v>
-      </c>
-      <c r="AD199" t="s">
-        <v>1267</v>
-      </c>
-      <c r="AE199" t="s">
-        <v>1268</v>
-      </c>
-      <c r="AF199" t="s">
-        <v>1269</v>
-      </c>
-      <c r="AG199" t="s">
+      <c r="AI199" t="s">
+        <v>1424</v>
+      </c>
+      <c r="AJ199" t="s">
         <v>1270</v>
       </c>
-      <c r="AH199" t="s">
-        <v>1424</v>
-      </c>
-      <c r="AI199" t="s">
-        <v>1425</v>
-      </c>
-      <c r="AJ199" t="s">
+      <c r="AK199" t="s">
         <v>1271</v>
       </c>
-      <c r="AK199" t="s">
+      <c r="AL199" t="s">
         <v>1272</v>
       </c>
-      <c r="AL199" t="s">
+      <c r="AM199" t="s">
         <v>1273</v>
       </c>
-      <c r="AM199" t="s">
+      <c r="AN199" t="s">
         <v>1274</v>
       </c>
-      <c r="AN199" t="s">
+      <c r="AO199" t="s">
         <v>1275</v>
       </c>
-      <c r="AO199" t="s">
+      <c r="AP199" t="s">
         <v>1276</v>
       </c>
-      <c r="AP199" t="s">
+      <c r="AQ199" t="s">
         <v>1277</v>
       </c>
-      <c r="AQ199" t="s">
+      <c r="AR199" t="s">
         <v>1278</v>
       </c>
-      <c r="AR199" t="s">
+      <c r="AS199" t="s">
         <v>1279</v>
       </c>
-      <c r="AS199" t="s">
+      <c r="AT199" t="s">
         <v>1280</v>
       </c>
-      <c r="AT199" t="s">
+      <c r="AU199" t="s">
         <v>1281</v>
       </c>
-      <c r="AU199" t="s">
+      <c r="AV199" t="s">
         <v>1282</v>
       </c>
-      <c r="AV199" t="s">
+      <c r="AW199" t="s">
         <v>1283</v>
       </c>
-      <c r="AW199" t="s">
+      <c r="AX199" t="s">
         <v>1284</v>
       </c>
-      <c r="AX199" t="s">
+      <c r="AY199" t="s">
         <v>1285</v>
       </c>
-      <c r="AY199" t="s">
+      <c r="AZ199" t="s">
         <v>1286</v>
       </c>
-      <c r="AZ199" t="s">
+      <c r="BA199" t="s">
         <v>1287</v>
       </c>
-      <c r="BA199" t="s">
+      <c r="BB199" t="s">
         <v>1288</v>
       </c>
-      <c r="BB199" t="s">
+      <c r="BC199" t="s">
         <v>1289</v>
       </c>
-      <c r="BC199" t="s">
+      <c r="BD199" t="s">
         <v>1290</v>
       </c>
-      <c r="BD199" t="s">
+      <c r="BE199" t="s">
         <v>1291</v>
       </c>
-      <c r="BE199" t="s">
+      <c r="BF199" t="s">
         <v>1292</v>
       </c>
-      <c r="BF199" t="s">
+      <c r="BG199" t="s">
         <v>1293</v>
       </c>
-      <c r="BG199" t="s">
+      <c r="BH199" t="s">
         <v>1294</v>
       </c>
-      <c r="BH199" t="s">
+      <c r="BI199" t="s">
         <v>1295</v>
       </c>
-      <c r="BI199" t="s">
+      <c r="BJ199" t="s">
         <v>1296</v>
       </c>
-      <c r="BJ199" t="s">
+      <c r="BK199" t="s">
         <v>1297</v>
       </c>
-      <c r="BK199" t="s">
+      <c r="BL199" t="s">
         <v>1298</v>
       </c>
-      <c r="BL199" t="s">
+      <c r="BM199" t="s">
         <v>1299</v>
       </c>
-      <c r="BM199" t="s">
+      <c r="BN199" t="s">
         <v>1300</v>
       </c>
-      <c r="BN199" t="s">
+      <c r="BO199" t="s">
         <v>1301</v>
       </c>
-      <c r="BO199" t="s">
+      <c r="BP199" t="s">
         <v>1302</v>
       </c>
-      <c r="BP199" t="s">
+      <c r="BQ199" t="s">
         <v>1303</v>
       </c>
-      <c r="BQ199" t="s">
+      <c r="BR199" t="s">
         <v>1304</v>
       </c>
-      <c r="BR199" t="s">
+      <c r="BS199" t="s">
         <v>1305</v>
       </c>
-      <c r="BS199" t="s">
+      <c r="BT199" t="s">
         <v>1306</v>
       </c>
-      <c r="BT199" t="s">
+      <c r="BU199" t="s">
         <v>1307</v>
       </c>
-      <c r="BU199" t="s">
+      <c r="BV199" t="s">
         <v>1308</v>
-      </c>
-      <c r="BV199" t="s">
-        <v>1309</v>
       </c>
     </row>
     <row r="200" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B200" t="s">
         <v>1</v>
@@ -11658,15 +11658,15 @@
         <v>148</v>
       </c>
       <c r="F200" t="s">
+        <v>1310</v>
+      </c>
+      <c r="G200" t="s">
         <v>1311</v>
-      </c>
-      <c r="G200" t="s">
-        <v>1312</v>
       </c>
     </row>
     <row r="201" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B201" t="s">
         <v>1</v>
@@ -11705,12 +11705,12 @@
         <v>465</v>
       </c>
       <c r="N201" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="202" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B202" t="s">
         <v>1</v>
@@ -11725,39 +11725,39 @@
         <v>148</v>
       </c>
       <c r="F202" t="s">
+        <v>1315</v>
+      </c>
+      <c r="G202" t="s">
         <v>1316</v>
       </c>
-      <c r="G202" t="s">
+      <c r="H202" t="s">
         <v>1317</v>
       </c>
-      <c r="H202" t="s">
+      <c r="I202" t="s">
         <v>1318</v>
       </c>
-      <c r="I202" t="s">
+      <c r="J202" t="s">
         <v>1319</v>
       </c>
-      <c r="J202" t="s">
+      <c r="K202" t="s">
         <v>1320</v>
       </c>
-      <c r="K202" t="s">
+      <c r="L202" t="s">
         <v>1321</v>
       </c>
-      <c r="L202" t="s">
+      <c r="M202" t="s">
         <v>1322</v>
       </c>
-      <c r="M202" t="s">
+      <c r="N202" t="s">
         <v>1323</v>
       </c>
-      <c r="N202" t="s">
+      <c r="O202" t="s">
         <v>1324</v>
-      </c>
-      <c r="O202" t="s">
-        <v>1325</v>
       </c>
     </row>
     <row r="203" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B203" t="s">
         <v>1</v>
@@ -11783,7 +11783,7 @@
     </row>
     <row r="204" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B204" t="s">
         <v>1</v>
@@ -11827,7 +11827,7 @@
     </row>
     <row r="205" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B205" t="s">
         <v>1</v>
@@ -11871,7 +11871,7 @@
     </row>
     <row r="206" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B206" t="s">
         <v>1</v>
@@ -11897,7 +11897,7 @@
     </row>
     <row r="207" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B207" t="s">
         <v>1</v>
@@ -11929,7 +11929,7 @@
     </row>
     <row r="208" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B208" t="s">
         <v>1</v>
@@ -11944,21 +11944,21 @@
         <v>148</v>
       </c>
       <c r="F208" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G208" t="s">
         <v>1034</v>
       </c>
-      <c r="G208" t="s">
+      <c r="H208" t="s">
         <v>1035</v>
       </c>
-      <c r="H208" t="s">
+      <c r="I208" t="s">
         <v>1036</v>
-      </c>
-      <c r="I208" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B209" t="s">
         <v>1</v>
@@ -12002,7 +12002,7 @@
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B210" t="s">
         <v>1</v>
@@ -12046,7 +12046,7 @@
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B211" t="s">
         <v>1</v>
@@ -12090,7 +12090,7 @@
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B212" t="s">
         <v>1</v>
@@ -12119,7 +12119,7 @@
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B213" t="s">
         <v>1</v>
@@ -12163,7 +12163,7 @@
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B214" t="s">
         <v>1</v>
@@ -12309,7 +12309,7 @@
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B218" t="s">
         <v>1</v>
@@ -12397,7 +12397,7 @@
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B220" t="s">
         <v>1</v>
@@ -12423,7 +12423,7 @@
     </row>
     <row r="221" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B221" t="s">
         <v>1</v>
@@ -12467,7 +12467,7 @@
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B222" t="s">
         <v>1</v>
@@ -12584,7 +12584,7 @@
     </row>
     <row r="225" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B225" t="s">
         <v>1</v>
@@ -12599,16 +12599,16 @@
         <v>148</v>
       </c>
       <c r="F225" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G225" t="s">
         <v>1034</v>
       </c>
-      <c r="G225" t="s">
+      <c r="H225" t="s">
         <v>1035</v>
       </c>
-      <c r="H225" t="s">
+      <c r="I225" t="s">
         <v>1036</v>
-      </c>
-      <c r="I225" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="226" spans="1:34" x14ac:dyDescent="0.3">
@@ -13006,7 +13006,7 @@
     </row>
     <row r="235" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B235" t="s">
         <v>1</v>
@@ -13018,15 +13018,15 @@
         <v>76</v>
       </c>
       <c r="E235" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F235" t="s">
         <v>1026</v>
-      </c>
-      <c r="F235" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="236" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B236" t="s">
         <v>1</v>
@@ -13035,16 +13035,16 @@
         <v>2</v>
       </c>
       <c r="D236" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E236" t="s">
         <v>1029</v>
       </c>
-      <c r="E236" t="s">
+      <c r="F236" t="s">
         <v>1030</v>
       </c>
-      <c r="F236" t="s">
+      <c r="G236" t="s">
         <v>1031</v>
-      </c>
-      <c r="G236" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="237" spans="1:34" x14ac:dyDescent="0.3">
@@ -13119,7 +13119,7 @@
     </row>
     <row r="239" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B239" t="s">
         <v>1</v>
@@ -13128,24 +13128,24 @@
         <v>577</v>
       </c>
       <c r="D239" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E239" t="s">
         <v>1342</v>
       </c>
-      <c r="E239" t="s">
+      <c r="F239" t="s">
         <v>1343</v>
       </c>
-      <c r="F239" t="s">
+      <c r="G239" t="s">
         <v>1344</v>
       </c>
-      <c r="G239" t="s">
+      <c r="H239" t="s">
         <v>1345</v>
-      </c>
-      <c r="H239" t="s">
-        <v>1346</v>
       </c>
     </row>
     <row r="240" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B240" t="s">
         <v>122</v>
@@ -13154,41 +13154,41 @@
         <v>123</v>
       </c>
       <c r="D240" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E240" t="s">
+        <v>1347</v>
+      </c>
+      <c r="F240" t="s">
         <v>1348</v>
       </c>
-      <c r="F240" t="s">
+      <c r="G240" t="s">
         <v>1349</v>
-      </c>
-      <c r="G240" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="241" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B241" t="s">
         <v>122</v>
       </c>
       <c r="C241" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D241" t="s">
         <v>1352</v>
       </c>
-      <c r="D241" t="s">
+      <c r="E241" t="s">
         <v>1353</v>
       </c>
-      <c r="E241" t="s">
+      <c r="F241" t="s">
         <v>1354</v>
-      </c>
-      <c r="F241" t="s">
-        <v>1355</v>
       </c>
     </row>
     <row r="242" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B242" t="s">
         <v>1</v>
@@ -13200,66 +13200,66 @@
         <v>394</v>
       </c>
       <c r="E242" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F242" t="s">
         <v>1357</v>
       </c>
-      <c r="F242" t="s">
+      <c r="G242" t="s">
         <v>1358</v>
       </c>
-      <c r="G242" t="s">
+      <c r="H242" t="s">
         <v>1359</v>
       </c>
-      <c r="H242" t="s">
+      <c r="I242" t="s">
         <v>1360</v>
       </c>
-      <c r="I242" t="s">
+      <c r="J242" t="s">
         <v>1361</v>
       </c>
-      <c r="J242" t="s">
+      <c r="K242" t="s">
         <v>1362</v>
       </c>
-      <c r="K242" t="s">
+      <c r="L242" t="s">
         <v>1363</v>
       </c>
-      <c r="L242" t="s">
+      <c r="M242" t="s">
         <v>1364</v>
       </c>
-      <c r="M242" t="s">
+      <c r="N242" t="s">
         <v>1365</v>
       </c>
-      <c r="N242" t="s">
+      <c r="O242" t="s">
         <v>1366</v>
       </c>
-      <c r="O242" t="s">
+      <c r="P242" t="s">
         <v>1367</v>
       </c>
-      <c r="P242" t="s">
+      <c r="Q242" t="s">
         <v>1368</v>
       </c>
-      <c r="Q242" t="s">
+      <c r="R242" t="s">
         <v>1369</v>
       </c>
-      <c r="R242" t="s">
+      <c r="S242" t="s">
         <v>1370</v>
       </c>
-      <c r="S242" t="s">
+      <c r="T242" t="s">
         <v>1371</v>
       </c>
-      <c r="T242" t="s">
+      <c r="U242" t="s">
         <v>1372</v>
       </c>
-      <c r="U242" t="s">
+      <c r="V242" t="s">
         <v>1373</v>
       </c>
-      <c r="V242" t="s">
+      <c r="W242" t="s">
         <v>1374</v>
-      </c>
-      <c r="W242" t="s">
-        <v>1375</v>
       </c>
     </row>
     <row r="243" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B243" t="s">
         <v>1</v>
@@ -13268,60 +13268,60 @@
         <v>577</v>
       </c>
       <c r="D243" t="s">
+        <v>963</v>
+      </c>
+      <c r="E243" t="s">
         <v>964</v>
       </c>
-      <c r="E243" t="s">
+      <c r="F243" t="s">
         <v>965</v>
       </c>
-      <c r="F243" t="s">
+      <c r="G243" t="s">
         <v>966</v>
       </c>
-      <c r="G243" t="s">
+      <c r="H243" t="s">
         <v>967</v>
       </c>
-      <c r="H243" t="s">
+      <c r="I243" t="s">
         <v>968</v>
       </c>
-      <c r="I243" t="s">
+      <c r="J243" t="s">
         <v>969</v>
       </c>
-      <c r="J243" t="s">
+      <c r="K243" t="s">
         <v>970</v>
       </c>
-      <c r="K243" t="s">
+      <c r="L243" t="s">
         <v>971</v>
       </c>
-      <c r="L243" t="s">
+      <c r="M243" t="s">
         <v>972</v>
       </c>
-      <c r="M243" t="s">
+      <c r="N243" t="s">
         <v>973</v>
       </c>
-      <c r="N243" t="s">
+      <c r="O243" t="s">
         <v>974</v>
       </c>
-      <c r="O243" t="s">
+      <c r="P243" t="s">
         <v>975</v>
       </c>
-      <c r="P243" t="s">
+      <c r="Q243" t="s">
         <v>976</v>
       </c>
-      <c r="Q243" t="s">
+      <c r="R243" t="s">
         <v>977</v>
       </c>
-      <c r="R243" t="s">
+      <c r="S243" t="s">
         <v>978</v>
       </c>
-      <c r="S243" t="s">
+      <c r="T243" t="s">
         <v>979</v>
-      </c>
-      <c r="T243" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="244" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B244" t="s">
         <v>1</v>
@@ -13330,21 +13330,21 @@
         <v>577</v>
       </c>
       <c r="D244" t="s">
+        <v>963</v>
+      </c>
+      <c r="E244" t="s">
         <v>964</v>
       </c>
-      <c r="E244" t="s">
-        <v>965</v>
-      </c>
       <c r="F244" t="s">
+        <v>988</v>
+      </c>
+      <c r="G244" t="s">
         <v>989</v>
-      </c>
-      <c r="G244" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="245" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B245" t="s">
         <v>1</v>
@@ -13359,21 +13359,21 @@
         <v>683</v>
       </c>
       <c r="F245" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G245" t="s">
         <v>1088</v>
       </c>
-      <c r="G245" t="s">
+      <c r="H245" t="s">
         <v>1089</v>
       </c>
-      <c r="H245" t="s">
+      <c r="I245" t="s">
         <v>1090</v>
-      </c>
-      <c r="I245" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="246" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B246" t="s">
         <v>1</v>
@@ -13388,30 +13388,30 @@
         <v>683</v>
       </c>
       <c r="F246" t="s">
+        <v>1376</v>
+      </c>
+      <c r="G246" t="s">
         <v>1377</v>
       </c>
-      <c r="G246" t="s">
+      <c r="H246" t="s">
         <v>1378</v>
       </c>
-      <c r="H246" t="s">
+      <c r="I246" t="s">
         <v>1379</v>
       </c>
-      <c r="I246" t="s">
+      <c r="J246" t="s">
         <v>1380</v>
       </c>
-      <c r="J246" t="s">
+      <c r="K246" t="s">
         <v>1381</v>
       </c>
-      <c r="K246" t="s">
+      <c r="L246" t="s">
         <v>1382</v>
-      </c>
-      <c r="L246" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="247" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B247" t="s">
         <v>1</v>
@@ -13426,15 +13426,15 @@
         <v>683</v>
       </c>
       <c r="F247" t="s">
+        <v>1384</v>
+      </c>
+      <c r="G247" t="s">
         <v>1385</v>
-      </c>
-      <c r="G247" t="s">
-        <v>1386</v>
       </c>
     </row>
     <row r="248" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B248" t="s">
         <v>1</v>
@@ -13449,7 +13449,7 @@
         <v>683</v>
       </c>
       <c r="F248" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="249" spans="1:23" x14ac:dyDescent="0.3">
@@ -13483,7 +13483,7 @@
     </row>
     <row r="250" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="B250" t="s">
         <v>1</v>
@@ -13498,7 +13498,7 @@
         <v>683</v>
       </c>
       <c r="F250" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="251" spans="1:23" x14ac:dyDescent="0.3">
@@ -13615,7 +13615,7 @@
     </row>
     <row r="253" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="B253" t="s">
         <v>1</v>
@@ -13671,7 +13671,7 @@
     </row>
     <row r="254" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B254" t="s">
         <v>1</v>
@@ -13727,7 +13727,7 @@
     </row>
     <row r="255" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B255" t="s">
         <v>1</v>
@@ -13745,45 +13745,45 @@
         <v>690</v>
       </c>
       <c r="G255" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="H255" t="s">
         <v>713</v>
       </c>
       <c r="I255" t="s">
+        <v>1050</v>
+      </c>
+      <c r="J255" t="s">
         <v>1051</v>
       </c>
-      <c r="J255" t="s">
+      <c r="K255" t="s">
         <v>1052</v>
-      </c>
-      <c r="K255" t="s">
-        <v>1053</v>
       </c>
       <c r="L255" t="s">
         <v>686</v>
       </c>
       <c r="M255" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N255" t="s">
         <v>1054</v>
       </c>
-      <c r="N255" t="s">
+      <c r="O255" t="s">
         <v>1055</v>
       </c>
-      <c r="O255" t="s">
+      <c r="P255" t="s">
         <v>1056</v>
       </c>
-      <c r="P255" t="s">
+      <c r="Q255" t="s">
         <v>1057</v>
       </c>
-      <c r="Q255" t="s">
+      <c r="R255" t="s">
         <v>1058</v>
-      </c>
-      <c r="R255" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="256" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="B256" t="s">
         <v>1</v>
@@ -13810,13 +13810,13 @@
         <v>689</v>
       </c>
       <c r="J256" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="K256" t="s">
         <v>686</v>
       </c>
       <c r="L256" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="M256" t="s">
         <v>684</v>
@@ -13836,7 +13836,7 @@
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B257" t="s">
         <v>1</v>
@@ -13892,7 +13892,7 @@
     </row>
     <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B258" t="s">
         <v>1</v>
@@ -13948,7 +13948,7 @@
     </row>
     <row r="259" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B259" t="s">
         <v>1</v>
@@ -13975,13 +13975,13 @@
         <v>689</v>
       </c>
       <c r="J259" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="K259" t="s">
         <v>686</v>
       </c>
       <c r="L259" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="M259" t="s">
         <v>684</v>
@@ -14001,7 +14001,7 @@
     </row>
     <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B260" t="s">
         <v>1</v>
@@ -14019,45 +14019,45 @@
         <v>690</v>
       </c>
       <c r="G260" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="H260" t="s">
         <v>713</v>
       </c>
       <c r="I260" t="s">
+        <v>1050</v>
+      </c>
+      <c r="J260" t="s">
         <v>1051</v>
       </c>
-      <c r="J260" t="s">
+      <c r="K260" t="s">
         <v>1052</v>
-      </c>
-      <c r="K260" t="s">
-        <v>1053</v>
       </c>
       <c r="L260" t="s">
         <v>686</v>
       </c>
       <c r="M260" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N260" t="s">
         <v>1054</v>
       </c>
-      <c r="N260" t="s">
+      <c r="O260" t="s">
         <v>1055</v>
       </c>
-      <c r="O260" t="s">
+      <c r="P260" t="s">
         <v>1056</v>
       </c>
-      <c r="P260" t="s">
+      <c r="Q260" t="s">
         <v>1057</v>
       </c>
-      <c r="Q260" t="s">
+      <c r="R260" t="s">
         <v>1058</v>
-      </c>
-      <c r="R260" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="261" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B261" t="s">
         <v>1</v>
@@ -14075,45 +14075,45 @@
         <v>690</v>
       </c>
       <c r="G261" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="H261" t="s">
         <v>713</v>
       </c>
       <c r="I261" t="s">
+        <v>1050</v>
+      </c>
+      <c r="J261" t="s">
         <v>1051</v>
       </c>
-      <c r="J261" t="s">
+      <c r="K261" t="s">
         <v>1052</v>
-      </c>
-      <c r="K261" t="s">
-        <v>1053</v>
       </c>
       <c r="L261" t="s">
         <v>686</v>
       </c>
       <c r="M261" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N261" t="s">
         <v>1054</v>
       </c>
-      <c r="N261" t="s">
+      <c r="O261" t="s">
         <v>1055</v>
       </c>
-      <c r="O261" t="s">
+      <c r="P261" t="s">
         <v>1056</v>
       </c>
-      <c r="P261" t="s">
+      <c r="Q261" t="s">
         <v>1057</v>
       </c>
-      <c r="Q261" t="s">
+      <c r="R261" t="s">
         <v>1058</v>
-      </c>
-      <c r="R261" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="B262" t="s">
         <v>1</v>
@@ -14140,13 +14140,13 @@
         <v>689</v>
       </c>
       <c r="J262" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="K262" t="s">
         <v>686</v>
       </c>
       <c r="L262" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="M262" t="s">
         <v>684</v>
@@ -14166,7 +14166,7 @@
     </row>
     <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="B263" t="s">
         <v>1</v>
@@ -14184,45 +14184,45 @@
         <v>690</v>
       </c>
       <c r="G263" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="H263" t="s">
         <v>713</v>
       </c>
       <c r="I263" t="s">
+        <v>1050</v>
+      </c>
+      <c r="J263" t="s">
         <v>1051</v>
       </c>
-      <c r="J263" t="s">
+      <c r="K263" t="s">
         <v>1052</v>
-      </c>
-      <c r="K263" t="s">
-        <v>1053</v>
       </c>
       <c r="L263" t="s">
         <v>686</v>
       </c>
       <c r="M263" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N263" t="s">
         <v>1054</v>
       </c>
-      <c r="N263" t="s">
+      <c r="O263" t="s">
         <v>1055</v>
       </c>
-      <c r="O263" t="s">
+      <c r="P263" t="s">
         <v>1056</v>
       </c>
-      <c r="P263" t="s">
+      <c r="Q263" t="s">
         <v>1057</v>
       </c>
-      <c r="Q263" t="s">
+      <c r="R263" t="s">
         <v>1058</v>
-      </c>
-      <c r="R263" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="B264" t="s">
         <v>1</v>
@@ -14234,27 +14234,27 @@
         <v>88</v>
       </c>
       <c r="E264" t="s">
+        <v>1394</v>
+      </c>
+      <c r="F264" t="s">
         <v>1395</v>
       </c>
-      <c r="F264" t="s">
+      <c r="G264" t="s">
         <v>1396</v>
       </c>
-      <c r="G264" t="s">
+      <c r="H264" t="s">
         <v>1397</v>
       </c>
-      <c r="H264" t="s">
+      <c r="I264" t="s">
         <v>1398</v>
       </c>
-      <c r="I264" t="s">
+      <c r="J264" t="s">
         <v>1399</v>
-      </c>
-      <c r="J264" t="s">
-        <v>1400</v>
       </c>
     </row>
     <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B265" t="s">
         <v>1</v>
@@ -14266,15 +14266,15 @@
         <v>88</v>
       </c>
       <c r="E265" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="F265" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B266" t="s">
         <v>1</v>
@@ -14283,30 +14283,30 @@
         <v>75</v>
       </c>
       <c r="D266" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E266" t="s">
         <v>1404</v>
       </c>
-      <c r="E266" t="s">
+      <c r="F266" t="s">
         <v>1405</v>
       </c>
-      <c r="F266" t="s">
+      <c r="G266" t="s">
         <v>1406</v>
       </c>
-      <c r="G266" t="s">
+      <c r="H266" t="s">
         <v>1407</v>
       </c>
-      <c r="H266" t="s">
+      <c r="I266" t="s">
         <v>1408</v>
       </c>
-      <c r="I266" t="s">
+      <c r="J266" t="s">
         <v>1409</v>
-      </c>
-      <c r="J266" t="s">
-        <v>1410</v>
       </c>
     </row>
     <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="B267" t="s">
         <v>1</v>
@@ -14318,16 +14318,16 @@
         <v>3</v>
       </c>
       <c r="E267" t="s">
+        <v>1411</v>
+      </c>
+      <c r="F267" t="s">
         <v>1412</v>
       </c>
-      <c r="F267" t="s">
+      <c r="G267" t="s">
         <v>1413</v>
       </c>
-      <c r="G267" t="s">
+      <c r="H267" t="s">
         <v>1414</v>
-      </c>
-      <c r="H267" t="s">
-        <v>1415</v>
       </c>
     </row>
     <row r="268" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>